<commit_message>
updating the source data..
</commit_message>
<xml_diff>
--- a/model-evals/llm_as_a_judge/data/source_data/data_user_system_prompt_version.xlsx
+++ b/model-evals/llm_as_a_judge/data/source_data/data_user_system_prompt_version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madhurpt/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CD32E45-65ED-0B40-A010-A473416966BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04BFCF3F-2061-8A42-8DD6-45218DEBA882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="1000" windowWidth="26260" windowHeight="15620" xr2:uid="{83B0547E-626D-4D47-81C3-ADEB83A05C56}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>user_input</t>
   </si>
   <si>
-    <t>dummy_model_response</t>
-  </si>
-  <si>
     <t>What is the Heisenberg uncertainty principle?</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>system_prompt</t>
+  </si>
+  <si>
+    <t>model_1</t>
   </si>
 </sst>
 </file>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603AF961-FDA2-8F46-ACE6-120B24AE456E}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="136" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,120 +608,120 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>